<commit_message>
today learn about wait and type of wait
</commit_message>
<xml_diff>
--- a/data/Testdata.xlsx
+++ b/data/Testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>firstname</t>
   </si>
@@ -43,6 +43,36 @@
   </si>
   <si>
     <t>lipu9888@gmail.com</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Sambalpur</t>
+  </si>
+  <si>
+    <t>ganjam</t>
+  </si>
+  <si>
+    <t>siddharth</t>
+  </si>
+  <si>
+    <t>nayak</t>
+  </si>
+  <si>
+    <t>siddharth@gamil.com</t>
+  </si>
+  <si>
+    <t>bhanjanagar</t>
+  </si>
+  <si>
+    <t>Rudar</t>
+  </si>
+  <si>
+    <t>sahoo</t>
+  </si>
+  <si>
+    <t>rudra477@gamil.com</t>
   </si>
 </sst>
 </file>
@@ -66,12 +96,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -87,9 +123,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -392,29 +429,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -424,8 +465,11 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -434,12 +478,45 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Today learn about how to data test in using excel
</commit_message>
<xml_diff>
--- a/data/Testdata.xlsx
+++ b/data/Testdata.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16485" windowHeight="6615" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="person" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginData" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>firstname</t>
   </si>
@@ -73,13 +73,40 @@
   </si>
   <si>
     <t>rudra477@gamil.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remark </t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>passowrod</t>
+  </si>
+  <si>
+    <t>mngr535530</t>
+  </si>
+  <si>
+    <t>pEsEraq</t>
+  </si>
+  <si>
+    <t>mngr5355304</t>
+  </si>
+  <si>
+    <t>pEsEraqh</t>
+  </si>
+  <si>
+    <t>pEsEraqy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +121,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF808080"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -123,10 +164,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -429,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +486,7 @@
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -454,8 +499,11 @@
       <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -469,7 +517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -482,8 +530,11 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -497,7 +548,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -509,6 +560,9 @@
       </c>
       <c r="D5" t="s">
         <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -524,13 +578,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>